<commit_message>
updating capstone projects file
</commit_message>
<xml_diff>
--- a/EKeeda DS June 2022/Projects/Capstone Projects/capstone_projects.xlsx
+++ b/EKeeda DS June 2022/Projects/Capstone Projects/capstone_projects.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
-    <t>Note: Each students is required to submit atleast one project from the following list of projects. However students are encouraged to try more than one projects as well.</t>
+    <t>Note: Each student is required to submit atleast one project from the following list of projects. However students are encouraged to try more than one projects.</t>
   </si>
   <si>
     <t>Sl. No.</t>
@@ -28908,11 +28908,11 @@
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B5:H5"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H10"/>
     <mergeCell ref="B11:H11"/>
-    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H12:H14"/>
     <mergeCell ref="B15:H15"/>
-    <mergeCell ref="H12:H14"/>
     <mergeCell ref="H16:H17"/>
   </mergeCells>
   <hyperlinks>

</xml_diff>